<commit_message>
Nota seminario 2.1 ssr
</commit_message>
<xml_diff>
--- a/4º/Notas Cuarto.xlsx
+++ b/4º/Notas Cuarto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ismael/Documents/GitHub/Ingenieria-Informatica/4º/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89D339B-7987-D741-8668-EE3D95837D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB819DAB-A0A8-7F42-8308-0634A36BDC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="1040" windowWidth="16840" windowHeight="21060" xr2:uid="{8C6909D8-F456-DC46-9AA4-5CA3DDF5E1C9}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{8C6909D8-F456-DC46-9AA4-5CA3DDF5E1C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -629,7 +629,7 @@
   <dimension ref="A4:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,7 +702,9 @@
       <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -711,7 +713,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="2">
         <f>B5*0.033+C5*0.033+D5*0.033+E5*0.033+F5*0.07+G5*0.033+H5*0.033+I5*0.065+J5*0.065</f>
-        <v>0.66</v>
+        <v>0.99</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -726,7 +728,7 @@
       </c>
       <c r="Q5" s="4">
         <f>P5+N5+K5</f>
-        <v>0.66</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Terminado trabajo 2 RCO
</commit_message>
<xml_diff>
--- a/4º/Notas Cuarto.xlsx
+++ b/4º/Notas Cuarto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Ingenieria-Informatica\4º\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D03DDB8-7E9E-4BB3-B4F9-0B3655127E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89642A5F-C983-4FB9-8CFF-94882BC9C35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="2355" windowWidth="21600" windowHeight="11295" xr2:uid="{8C6909D8-F456-DC46-9AA4-5CA3DDF5E1C9}"/>
   </bookViews>
@@ -626,7 +626,7 @@
   <dimension ref="A4:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>